<commit_message>
mod @20171226 by yxq
</commit_message>
<xml_diff>
--- a/xboost/com.xboost.business/src/main/webapp/static/excelTemplate/Test - Settings - Demands.xlsx
+++ b/xboost/com.xboost.business/src/main/webapp/static/excelTemplate/Test - Settings - Demands.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView windowWidth="19104" windowHeight="7787"/>
   </bookViews>
   <sheets>
     <sheet name="“Demands” Settings" sheetId="4" r:id="rId1"/>
@@ -49,10 +49,10 @@
     <t>755A</t>
   </si>
   <si>
-    <t>10:00:00</t>
+    <t>14:00:00</t>
   </si>
   <si>
-    <t>12:00:00</t>
+    <t>16:00:00</t>
   </si>
   <si>
     <t>755AA</t>
@@ -100,10 +100,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="h:mm;@"/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -129,8 +129,70 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -144,23 +206,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -190,30 +238,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -226,7 +251,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
@@ -236,31 +260,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -275,7 +275,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,7 +335,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -299,13 +359,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -317,31 +371,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -353,37 +383,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,13 +419,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,43 +443,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,41 +484,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -538,11 +523,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -567,17 +558,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -587,10 +587,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -599,133 +599,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1060,20 +1060,20 @@
   <sheetPr/>
   <dimension ref="A1:I197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F197"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="6.425" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.1416666666667" customWidth="1"/>
+    <col min="1" max="2" width="6.42592592592593" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.1388888888889" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.5666666666667" customWidth="1"/>
-    <col min="6" max="6" width="17.7083333333333" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.2833333333333" customWidth="1"/>
-    <col min="8" max="8" width="12.425" customWidth="1"/>
-    <col min="9" max="9" width="12.2833333333333" customWidth="1"/>
+    <col min="5" max="5" width="11.5648148148148" customWidth="1"/>
+    <col min="6" max="6" width="17.712962962963" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.287037037037" customWidth="1"/>
+    <col min="8" max="8" width="12.4259259259259" customWidth="1"/>
+    <col min="9" max="9" width="12.287037037037" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:9">

</xml_diff>